<commit_message>
Adding Architecture Design Doc and updated time log
</commit_message>
<xml_diff>
--- a/Phase 2 Documentation/Phase Two Time Log.xlsx
+++ b/Phase 2 Documentation/Phase Two Time Log.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blakeman/Documents/Planr/Phase 2 Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F845AA82-D196-0A41-A48A-4E981CBF9BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57790F56-74D3-1344-91BB-CF0223969F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{52085EF4-1DF1-914B-8651-54C060764F1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -54,13 +54,16 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Phase 2 Requirements</t>
-  </si>
-  <si>
-    <t>Investigating Phase 2 Requirements. Setting up documentation for Phase 2.</t>
-  </si>
-  <si>
     <t>System Architecture Document</t>
+  </si>
+  <si>
+    <t>Started System Architecture Document.</t>
+  </si>
+  <si>
+    <t>UML Diagram</t>
+  </si>
+  <si>
+    <t>Creating UML class diagrams for architecture document.</t>
   </si>
 </sst>
 </file>
@@ -68,8 +71,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="168" formatCode="h:mm:ss;@"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="h:mm:ss;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -112,8 +115,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5A7878-C821-8C47-B0EE-4E8CD483D98D}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -465,13 +468,17 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>44470</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+        <v>44490</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.74305555555555547</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.75</v>
+      </c>
       <c r="D2" s="4">
-        <f t="shared" ref="D2:D8" si="0">C2-B2</f>
-        <v>0</v>
+        <f>C2-B2</f>
+        <v>6.9444444444445308E-3</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -481,86 +488,53 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>44472</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="D3" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C3-B3</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>44473</v>
-      </c>
+      <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>44478</v>
-      </c>
+      <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>44480</v>
-      </c>
+      <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>44483</v>
-      </c>
+      <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="4">
-        <f>C7-B7</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>44487</v>
-      </c>
+      <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>44490</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0.74305555555555547</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="4">
-        <f>C9-B9</f>
-        <v>-0.74305555555555547</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
@@ -618,42 +592,7 @@
       <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
       <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add time for Phase Two Time Log
</commit_message>
<xml_diff>
--- a/Phase 2 Documentation/Phase Two Time Log.xlsx
+++ b/Phase 2 Documentation/Phase Two Time Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blakeman/Documents/Planr/Phase 2 Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57790F56-74D3-1344-91BB-CF0223969F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FDE7C8-6CD0-494E-B5DF-296334DE11D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{52085EF4-1DF1-914B-8651-54C060764F1A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>Creating UML class diagrams for architecture document.</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>Reworking UML class models</t>
+  </si>
+  <si>
+    <t>Continued work on UML class models.</t>
   </si>
 </sst>
 </file>
@@ -434,7 +443,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -507,39 +516,91 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+      <c r="A4" s="2">
+        <v>44491</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.71875</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" ref="D4:D10" si="0">C4-B4</f>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="A5" s="2">
+        <v>44493</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.53125</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="D5" s="4">
+        <f>C5-B5</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
+      <c r="D9" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
+      <c r="D10" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>

</xml_diff>

<commit_message>
Updated models and implemented new class
Updated time log as well
</commit_message>
<xml_diff>
--- a/Phase 2 Documentation/Phase Two Time Log.xlsx
+++ b/Phase 2 Documentation/Phase Two Time Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blakeman/Documents/Planr/Phase 2 Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FDE7C8-6CD0-494E-B5DF-296334DE11D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6045B06F-8BB8-1441-9DDF-56D4DD5AE328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{52085EF4-1DF1-914B-8651-54C060764F1A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Continued work on UML class models.</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Writing code from the UML diagrams.</t>
   </si>
 </sst>
 </file>
@@ -442,9 +448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5A7878-C821-8C47-B0EE-4E8CD483D98D}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -558,21 +562,43 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="A6" s="2">
+        <v>44495</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.875</v>
+      </c>
       <c r="D6" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.9145833333333333</v>
+      </c>
       <c r="D7" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.9583333333333304E-2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated code and time log
</commit_message>
<xml_diff>
--- a/Phase 2 Documentation/Phase Two Time Log.xlsx
+++ b/Phase 2 Documentation/Phase Two Time Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blakeman/Documents/Planr/Phase 2 Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6045B06F-8BB8-1441-9DDF-56D4DD5AE328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFE214E-EBBB-0942-A4DB-2A21434C7584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{52085EF4-1DF1-914B-8651-54C060764F1A}"/>
+    <workbookView xWindow="23560" yWindow="11860" windowWidth="27640" windowHeight="16940" xr2:uid="{52085EF4-1DF1-914B-8651-54C060764F1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Writing code from the UML diagrams.</t>
+  </si>
+  <si>
+    <t>Writing code from the UML diagrams. Specifically working on planning algorithm.</t>
+  </si>
+  <si>
+    <t>Writing code from the UML diagrams. Specifically working on planning algorithm. Also updated Vision doc to add team velocity input.</t>
   </si>
 </sst>
 </file>
@@ -448,7 +454,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5A7878-C821-8C47-B0EE-4E8CD483D98D}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -530,7 +538,7 @@
         <v>0.71875</v>
       </c>
       <c r="D4" s="4">
-        <f t="shared" ref="D4:D10" si="0">C4-B4</f>
+        <f t="shared" ref="D4:D11" si="0">C4-B4</f>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="E4" t="s">
@@ -602,36 +610,88 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="A8" s="2">
+        <v>44497</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.46875</v>
+      </c>
       <c r="D8" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.375E-2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="2">
+        <v>44498</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.46875</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.5</v>
+      </c>
       <c r="D9" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="A10" s="2">
+        <v>44499</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="D10" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.14583333333333337</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="A11" s="2">
+        <v>44501</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="0"/>
+        <v>0.37500000000000006</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>

</xml_diff>

<commit_message>
Updating documentation adding Phase 2 Presentation
</commit_message>
<xml_diff>
--- a/Phase 2 Documentation/Phase Two Time Log.xlsx
+++ b/Phase 2 Documentation/Phase Two Time Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blakeman/Documents/Planr/Phase 2 Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFE214E-EBBB-0942-A4DB-2A21434C7584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EE0766-DD35-A141-9D6E-4EFF68EB2D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23560" yWindow="11860" windowWidth="27640" windowHeight="16940" xr2:uid="{52085EF4-1DF1-914B-8651-54C060764F1A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{52085EF4-1DF1-914B-8651-54C060764F1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -85,6 +85,18 @@
   </si>
   <si>
     <t>Writing code from the UML diagrams. Specifically working on planning algorithm. Also updated Vision doc to add team velocity input.</t>
+  </si>
+  <si>
+    <t>Code cleanup</t>
+  </si>
+  <si>
+    <t>Cleaning up code for presentation.</t>
+  </si>
+  <si>
+    <t>Presentation Prep</t>
+  </si>
+  <si>
+    <t>Preparing for Phase 2 Presentation</t>
   </si>
 </sst>
 </file>
@@ -455,7 +467,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -538,7 +550,7 @@
         <v>0.71875</v>
       </c>
       <c r="D4" s="4">
-        <f t="shared" ref="D4:D11" si="0">C4-B4</f>
+        <f t="shared" ref="D4:D12" si="0">C4-B4</f>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="E4" t="s">
@@ -694,14 +706,38 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="A12" s="2">
+        <v>44502</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="0"/>
+        <v>3.819444444444442E-2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
+      <c r="B13" s="3">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="C13" s="3"/>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>

</xml_diff>

<commit_message>
Update presentation and time log
</commit_message>
<xml_diff>
--- a/Phase 2 Documentation/Phase Two Time Log.xlsx
+++ b/Phase 2 Documentation/Phase Two Time Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blakeman/Documents/Planr/Phase 2 Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88572BBC-0C0C-214C-BA61-E63080E54C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3429AA-83D8-394D-89A4-C9B7D150CD7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-51200" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{52085EF4-1DF1-914B-8651-54C060764F1A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>Creating boilerplate classes from UML.</t>
+  </si>
+  <si>
+    <t>Test Plan Document</t>
+  </si>
+  <si>
+    <t>Creating Test Plan Document</t>
   </si>
 </sst>
 </file>
@@ -153,12 +159,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5A7878-C821-8C47-B0EE-4E8CD483D98D}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,7 +627,7 @@
         <v>0.71875</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" ref="D7:D16" si="1">C7-B7</f>
+        <f t="shared" ref="D7:D18" si="1">C7-B7</f>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="E7" t="s">
@@ -822,7 +829,13 @@
       <c r="B17" s="3">
         <v>0.79166666666666663</v>
       </c>
-      <c r="C17" s="3"/>
+      <c r="C17" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="D17" s="4">
+        <f t="shared" si="1"/>
+        <v>8.333333333333337E-2</v>
+      </c>
       <c r="E17" t="s">
         <v>19</v>
       </c>
@@ -832,8 +845,22 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="B18" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" si="1"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
@@ -868,6 +895,9 @@
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" s="3"/>
     </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D33" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>